<commit_message>
Update MN and GA
</commit_message>
<xml_diff>
--- a/rules/map_sample_types.xlsx
+++ b/rules/map_sample_types.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Usbtl-serv-pdc1\Users\nmirasol\My Documents\Misc\sti-rules\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FE1816-618C-4988-8E9F-3F3C148AB0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF66CFC-DEE9-443C-BA34-B46DBE2820BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-3600" windowWidth="16440" windowHeight="29040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="69">
   <si>
     <t>Rectal</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>urinary</t>
   </si>
 </sst>
 </file>
@@ -1516,7 +1519,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,7 +1652,7 @@
         <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1666,7 +1669,7 @@
         <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1683,7 +1686,7 @@
         <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1700,7 +1703,7 @@
         <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add first draft of LA
</commit_message>
<xml_diff>
--- a/rules/map_sample_types.xlsx
+++ b/rules/map_sample_types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Usbtl-serv-pdc1\Users\nmirasol\My Documents\Misc\sti-rules\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF66CFC-DEE9-443C-BA34-B46DBE2820BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5A1278-FF4C-423A-9FD8-C215B2CFD8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Default" sheetId="1" r:id="rId1"/>
     <sheet name="CA" sheetId="2" r:id="rId2"/>
     <sheet name="IL" sheetId="3" r:id="rId3"/>
-    <sheet name="MN" sheetId="4" r:id="rId4"/>
+    <sheet name="LA" sheetId="5" r:id="rId4"/>
+    <sheet name="MN" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="71">
   <si>
     <t>Rectal</t>
   </si>
@@ -246,6 +247,12 @@
   </si>
   <si>
     <t>urinary</t>
+  </si>
+  <si>
+    <t>urogenital</t>
+  </si>
+  <si>
+    <t>oral</t>
   </si>
 </sst>
 </file>
@@ -1515,11 +1522,305 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{359080B4-7E71-4926-AB9F-C89D037B1987}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE2BAD1-CED3-486B-80F5-35C96CA54C12}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="A1:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>